<commit_message>
Program Post and Get REquest
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestDataExcel.xlsx
+++ b/src/test/resources/TestData/TestDataExcel.xlsx
@@ -3,22 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arvin\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2432C211-174E-46EC-8880-372E61E8867A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{35D2E3BD-7B3B-47A5-A12F-03A2F5BA9141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7448738B-910C-4297-A717-1563F2DCD82C}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7448738B-910C-4297-A717-1563F2DCD82C}"/>
   </bookViews>
   <sheets>
     <sheet name="UserLogin" sheetId="1" r:id="rId1"/>
-    <sheet name="Program" sheetId="2" r:id="rId2"/>
+    <sheet name="ProgramController" sheetId="2" r:id="rId2"/>
     <sheet name="Batch" sheetId="3" r:id="rId3"/>
     <sheet name="User" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:U6"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>Email</t>
   </si>
@@ -46,13 +42,70 @@
   </si>
   <si>
     <t>SDET</t>
+  </si>
+  <si>
+    <t>programDescription</t>
+  </si>
+  <si>
+    <t>programName</t>
+  </si>
+  <si>
+    <t>programStatus</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>March24-APICoders-2</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>March24-APICoders-1</t>
+  </si>
+  <si>
+    <t>testinvalid</t>
+  </si>
+  <si>
+    <t>$$$$</t>
+  </si>
+  <si>
+    <t>MN1111</t>
+  </si>
+  <si>
+    <t>March24-APICoders-3</t>
+  </si>
+  <si>
+    <t>inactive</t>
+  </si>
+  <si>
+    <t>March24-APICoders-4</t>
+  </si>
+  <si>
+    <t>March24-APICoders-5</t>
+  </si>
+  <si>
+    <t>March24-APICoders-6</t>
+  </si>
+  <si>
+    <t>activate</t>
+  </si>
+  <si>
+    <t>March24-APICoders-7</t>
+  </si>
+  <si>
+    <t>deactivate</t>
+  </si>
+  <si>
+    <t>name invalid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,6 +121,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -77,7 +143,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -85,14 +151,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -410,7 +500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44E3F3DD-EB8E-4C2A-996E-E0B59421C503}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -463,12 +553,163 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A9043B-614D-43BA-945E-6B63D978CE4D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>1234</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>